<commit_message>
modification des fichiers excel pour expliquer a un membre le fonctionnement
</commit_message>
<xml_diff>
--- a/ent_infoConnect/bd_etudiant.xlsx
+++ b/ent_infoConnect/bd_etudiant.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t xml:space="preserve">matricule</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t xml:space="preserve">Pashler.Jelene@facsciences-uy1.cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21T2284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ivan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kamdem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ivan.kamdem@facsciences-uy1.cm</t>
   </si>
 </sst>
 </file>
@@ -312,16 +324,16 @@
   <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.35546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="0" width="8.74"/>
   </cols>
@@ -472,6 +484,24 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -569,6 +599,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="sorelle.tchami@facsciences-uy1.cm"/>
+    <hyperlink ref="E8" r:id="rId2" display="ivan.kamdem@facsciences-uy1.cm"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>